<commit_message>
start shift event in k7 and send message telegram
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -19,12 +19,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data_Separation!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Settings!$A$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>Имя</t>
   </si>
@@ -153,6 +153,21 @@
   </si>
   <si>
     <t xml:space="preserve">сам иб </t>
+  </si>
+  <si>
+    <t>7040168084:AAHV6YxGTIpaFKsU7kKY6K5LjOKlNXcQW5U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Токен от бота в телеграм </t>
+  </si>
+  <si>
+    <t>Token_Telegram</t>
+  </si>
+  <si>
+    <t>IdChat_Telegram</t>
+  </si>
+  <si>
+    <t>id чата для рассылки уведомлений</t>
   </si>
 </sst>
 </file>
@@ -572,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E544"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -767,9 +782,27 @@
       <c r="D18" s="8"/>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="D19" s="8"/>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="10">
+        <v>748500486</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="D20" s="8"/>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>